<commit_message>
new changes in Connection DB file
</commit_message>
<xml_diff>
--- a/sel_training/records.xlsx
+++ b/sel_training/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="5535"/>
   </bookViews>
   <sheets>
     <sheet name="emp" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>ishan</t>
   </si>
@@ -463,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,6 +815,57 @@
         <v>57000</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>57000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>